<commit_message>
Updated DB connections to use DATABASE_URL for Render
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\JobmatchV2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFDC7AF2-BDAD-4CF9-ABD0-4DCBD2D84776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9646507F-F7B9-4745-BDE8-A033A036CA32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9960" yWindow="225" windowWidth="9870" windowHeight="10515" tabRatio="628" xr2:uid="{73A35279-5B22-4D14-8EE2-87191DD8957A}"/>
   </bookViews>
@@ -567,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ADEF93B-046F-443C-8AE5-F2920FD40003}">
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,9 +782,33 @@
         <v>34</v>
       </c>
     </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <v>1400</v>
+      </c>
+      <c r="L8">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K9">
+        <v>247</v>
+      </c>
+      <c r="L9">
+        <v>70</v>
+      </c>
+    </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>0.08</v>
+      </c>
+      <c r="K10" s="5">
+        <f>K9/K8</f>
+        <v>0.17642857142857143</v>
+      </c>
+      <c r="L10" s="5">
+        <f>(L9-L8)/L8</f>
+        <v>-0.38596491228070173</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add detailed logging for registration errors
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\JobmatchV2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9646507F-F7B9-4745-BDE8-A033A036CA32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FAE93D2-82F2-444D-919F-B8A93FDB1FCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9960" yWindow="225" windowWidth="9870" windowHeight="10515" tabRatio="628" xr2:uid="{73A35279-5B22-4D14-8EE2-87191DD8957A}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -43,9 +43,6 @@
     <t>amitabh@gmail.com</t>
   </si>
   <si>
-    <t>Amit@bh020525</t>
-  </si>
-  <si>
     <t>Hrithik</t>
   </si>
   <si>
@@ -182,6 +179,18 @@
   </si>
   <si>
     <t>extra for induction</t>
+  </si>
+  <si>
+    <t>Amit$bh020525</t>
+  </si>
+  <si>
+    <t>Katrina</t>
+  </si>
+  <si>
+    <t>katrina@gmail.com</t>
+  </si>
+  <si>
+    <t>Katy$080525</t>
   </si>
 </sst>
 </file>
@@ -239,7 +248,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
@@ -248,6 +257,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -567,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ADEF93B-046F-443C-8AE5-F2920FD40003}">
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,22 +609,22 @@
         <v>1500</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I1" s="4">
         <v>10</v>
       </c>
       <c r="J1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -624,11 +634,11 @@
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
+      <c r="C2" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F2">
         <f>J2/G2</f>
@@ -663,16 +673,16 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F4" si="0">J3/G3</f>
@@ -707,16 +717,16 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
@@ -751,38 +761,47 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" t="s">
         <v>28</v>
-      </c>
-      <c r="C5" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" t="s">
         <v>33</v>
       </c>
-      <c r="C7" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" t="s">
+        <v>54</v>
+      </c>
       <c r="K8">
         <v>1400</v>
       </c>
@@ -982,7 +1001,7 @@
         <v>546000</v>
       </c>
       <c r="K16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L16">
         <v>500</v>
@@ -995,7 +1014,7 @@
         <v>700</v>
       </c>
       <c r="O16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -1023,7 +1042,7 @@
         <v>87379</v>
       </c>
       <c r="K17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L17">
         <v>500</v>
@@ -1061,7 +1080,7 @@
         <v>870705</v>
       </c>
       <c r="K18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L18">
         <v>500</v>
@@ -1103,7 +1122,7 @@
         <v>15</v>
       </c>
       <c r="K19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L19">
         <v>500</v>
@@ -1303,12 +1322,12 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{4D886C74-7A58-49F4-8648-E916B1C797F8}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{8A98BE03-4FC1-44A2-9563-33ACE231306F}"/>
-    <hyperlink ref="B3" r:id="rId3" xr:uid="{BFAC1C57-995A-41F5-A055-C6AF0781F721}"/>
-    <hyperlink ref="B4" r:id="rId4" xr:uid="{91487797-136A-40DF-9DE9-66B358046DF4}"/>
-    <hyperlink ref="B5" r:id="rId5" xr:uid="{B4144595-B91F-4B74-AA0F-578F886134AA}"/>
-    <hyperlink ref="B6" r:id="rId6" xr:uid="{2E082BAA-FACB-49ED-8DE6-E44DE0493730}"/>
-    <hyperlink ref="B7" r:id="rId7" xr:uid="{04A41F48-7108-482E-884C-C56970220445}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{BFAC1C57-995A-41F5-A055-C6AF0781F721}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{91487797-136A-40DF-9DE9-66B358046DF4}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{B4144595-B91F-4B74-AA0F-578F886134AA}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{2E082BAA-FACB-49ED-8DE6-E44DE0493730}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{04A41F48-7108-482E-884C-C56970220445}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{983A4C4F-3674-464D-8443-3CDD4BF19090}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1340,68 +1359,68 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
         <v>15</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" t="s">
         <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" t="s">
         <v>22</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" t="s">
         <v>25</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" t="s">
         <v>36</v>
-      </c>
-      <c r="C7" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>